<commit_message>
list HoaDon: bind {GiamtrubaoHiem}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon_Gara.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon_Gara.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Tên khách hàng</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Giá trị sau trả</t>
+  </si>
+  <si>
+    <t>Giảm trừ Bảo hiểm</t>
   </si>
 </sst>
 </file>
@@ -286,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -381,6 +384,9 @@
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -711,12 +717,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR33"/>
+  <dimension ref="A1:AS33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,66 +748,68 @@
     <col min="24" max="24" width="19.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="25" max="27" width="19.140625" style="7" customWidth="1"/>
     <col min="28" max="28" width="31" style="7" customWidth="1"/>
-    <col min="29" max="29" width="22" style="7" customWidth="1"/>
-    <col min="30" max="30" width="23.42578125" style="7" customWidth="1"/>
-    <col min="31" max="31" width="24.140625" style="7" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" style="7" customWidth="1"/>
-    <col min="33" max="33" width="25.7109375" style="7" customWidth="1"/>
-    <col min="34" max="40" width="19.140625" style="7" customWidth="1"/>
-    <col min="41" max="42" width="18.140625" style="7" customWidth="1"/>
-    <col min="43" max="43" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="1"/>
+    <col min="29" max="29" width="29.7109375" style="7" customWidth="1"/>
+    <col min="30" max="30" width="22" style="7" customWidth="1"/>
+    <col min="31" max="31" width="23.42578125" style="7" customWidth="1"/>
+    <col min="32" max="32" width="24.140625" style="7" customWidth="1"/>
+    <col min="33" max="33" width="22.5703125" style="7" customWidth="1"/>
+    <col min="34" max="34" width="25.7109375" style="7" customWidth="1"/>
+    <col min="35" max="41" width="19.140625" style="7" customWidth="1"/>
+    <col min="42" max="43" width="18.140625" style="7" customWidth="1"/>
+    <col min="44" max="44" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="38"/>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="38"/>
-      <c r="AO1" s="38"/>
-      <c r="AP1" s="38"/>
-      <c r="AQ1" s="38"/>
-      <c r="AR1" s="5"/>
-    </row>
-    <row r="2" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="39"/>
+      <c r="AI1" s="39"/>
+      <c r="AJ1" s="39"/>
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="39"/>
+      <c r="AM1" s="39"/>
+      <c r="AN1" s="39"/>
+      <c r="AO1" s="39"/>
+      <c r="AP1" s="39"/>
+      <c r="AQ1" s="39"/>
+      <c r="AR1" s="39"/>
+      <c r="AS1" s="5"/>
+    </row>
+    <row r="2" spans="1:45" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="22"/>
       <c r="C2" s="18"/>
@@ -830,24 +838,25 @@
       <c r="Z2" s="37"/>
       <c r="AA2" s="33"/>
       <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
+      <c r="AC2" s="38"/>
       <c r="AD2" s="36"/>
       <c r="AE2" s="36"/>
       <c r="AF2" s="36"/>
-      <c r="AG2" s="33"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="33"/>
-      <c r="AI2" s="35"/>
-      <c r="AJ2" s="25"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="35"/>
       <c r="AK2" s="25"/>
       <c r="AL2" s="25"/>
-      <c r="AM2" s="35"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="18"/>
-      <c r="AR2" s="5"/>
-    </row>
-    <row r="3" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="35"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="23"/>
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="18"/>
+      <c r="AS2" s="5"/>
+    </row>
+    <row r="3" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>13</v>
       </c>
@@ -878,24 +887,25 @@
       <c r="Z3" s="37"/>
       <c r="AA3" s="33"/>
       <c r="AB3" s="36"/>
-      <c r="AC3" s="36"/>
+      <c r="AC3" s="38"/>
       <c r="AD3" s="36"/>
       <c r="AE3" s="36"/>
       <c r="AF3" s="36"/>
-      <c r="AG3" s="33"/>
+      <c r="AG3" s="36"/>
       <c r="AH3" s="33"/>
-      <c r="AI3" s="35"/>
-      <c r="AJ3" s="25"/>
+      <c r="AI3" s="33"/>
+      <c r="AJ3" s="35"/>
       <c r="AK3" s="25"/>
       <c r="AL3" s="25"/>
-      <c r="AM3" s="35"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="23"/>
-      <c r="AP3" s="34"/>
-      <c r="AQ3" s="18"/>
-      <c r="AR3" s="5"/>
-    </row>
-    <row r="4" spans="1:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM3" s="25"/>
+      <c r="AN3" s="35"/>
+      <c r="AO3" s="25"/>
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="34"/>
+      <c r="AR3" s="18"/>
+      <c r="AS3" s="5"/>
+    </row>
+    <row r="4" spans="1:45" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
@@ -926,24 +936,25 @@
       <c r="Z4" s="37"/>
       <c r="AA4" s="33"/>
       <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
+      <c r="AC4" s="38"/>
       <c r="AD4" s="36"/>
       <c r="AE4" s="36"/>
       <c r="AF4" s="36"/>
-      <c r="AG4" s="33"/>
+      <c r="AG4" s="36"/>
       <c r="AH4" s="33"/>
-      <c r="AI4" s="35"/>
-      <c r="AJ4" s="25"/>
+      <c r="AI4" s="33"/>
+      <c r="AJ4" s="35"/>
       <c r="AK4" s="25"/>
       <c r="AL4" s="25"/>
-      <c r="AM4" s="35"/>
-      <c r="AN4" s="25"/>
-      <c r="AO4" s="23"/>
-      <c r="AP4" s="34"/>
-      <c r="AQ4" s="18"/>
-      <c r="AR4" s="5"/>
-    </row>
-    <row r="5" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM4" s="25"/>
+      <c r="AN4" s="35"/>
+      <c r="AO4" s="25"/>
+      <c r="AP4" s="23"/>
+      <c r="AQ4" s="34"/>
+      <c r="AR4" s="18"/>
+      <c r="AS4" s="5"/>
+    </row>
+    <row r="5" spans="1:45" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -985,8 +996,9 @@
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
-    </row>
-    <row r="6" spans="1:44" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AR5" s="1"/>
+    </row>
+    <row r="6" spans="1:45" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1072,52 +1084,55 @@
         <v>39</v>
       </c>
       <c r="AC6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AD6" s="4" t="s">
+      <c r="AE6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AE6" s="4" t="s">
+      <c r="AF6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AF6" s="4" t="s">
+      <c r="AG6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AG6" s="4" t="s">
+      <c r="AH6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AH6" s="4" t="s">
+      <c r="AI6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AI6" s="4" t="s">
+      <c r="AJ6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AJ6" s="4" t="s">
+      <c r="AK6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AK6" s="4" t="s">
+      <c r="AL6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AL6" s="4" t="s">
+      <c r="AM6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AM6" s="4" t="s">
+      <c r="AN6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AN6" s="4" t="s">
+      <c r="AO6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AO6" s="4" t="s">
+      <c r="AP6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AP6" s="4" t="s">
+      <c r="AQ6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AQ6" s="10" t="s">
+      <c r="AR6" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="16"/>
@@ -1160,9 +1175,10 @@
       <c r="AN7" s="6"/>
       <c r="AO7" s="6"/>
       <c r="AP7" s="6"/>
-      <c r="AQ7" s="13"/>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="13"/>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="16"/>
@@ -1205,9 +1221,10 @@
       <c r="AN8" s="6"/>
       <c r="AO8" s="6"/>
       <c r="AP8" s="6"/>
-      <c r="AQ8" s="13"/>
-    </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="13"/>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="16"/>
@@ -1250,9 +1267,10 @@
       <c r="AN9" s="6"/>
       <c r="AO9" s="6"/>
       <c r="AP9" s="6"/>
-      <c r="AQ9" s="13"/>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="13"/>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="16"/>
@@ -1295,9 +1313,10 @@
       <c r="AN10" s="6"/>
       <c r="AO10" s="6"/>
       <c r="AP10" s="6"/>
-      <c r="AQ10" s="13"/>
-    </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="13"/>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="16"/>
@@ -1340,9 +1359,10 @@
       <c r="AN11" s="6"/>
       <c r="AO11" s="6"/>
       <c r="AP11" s="6"/>
-      <c r="AQ11" s="13"/>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ11" s="6"/>
+      <c r="AR11" s="13"/>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="16"/>
@@ -1385,9 +1405,10 @@
       <c r="AN12" s="6"/>
       <c r="AO12" s="6"/>
       <c r="AP12" s="6"/>
-      <c r="AQ12" s="13"/>
-    </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ12" s="6"/>
+      <c r="AR12" s="13"/>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="16"/>
@@ -1430,9 +1451,10 @@
       <c r="AN13" s="6"/>
       <c r="AO13" s="6"/>
       <c r="AP13" s="6"/>
-      <c r="AQ13" s="13"/>
-    </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ13" s="6"/>
+      <c r="AR13" s="13"/>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="16"/>
@@ -1475,9 +1497,10 @@
       <c r="AN14" s="6"/>
       <c r="AO14" s="6"/>
       <c r="AP14" s="6"/>
-      <c r="AQ14" s="13"/>
-    </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ14" s="6"/>
+      <c r="AR14" s="13"/>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="16"/>
@@ -1520,9 +1543,10 @@
       <c r="AN15" s="6"/>
       <c r="AO15" s="6"/>
       <c r="AP15" s="6"/>
-      <c r="AQ15" s="13"/>
-    </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ15" s="6"/>
+      <c r="AR15" s="13"/>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="16"/>
@@ -1565,9 +1589,10 @@
       <c r="AN16" s="6"/>
       <c r="AO16" s="6"/>
       <c r="AP16" s="6"/>
-      <c r="AQ16" s="13"/>
-    </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ16" s="6"/>
+      <c r="AR16" s="13"/>
+    </row>
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="16"/>
@@ -1610,9 +1635,10 @@
       <c r="AN17" s="6"/>
       <c r="AO17" s="6"/>
       <c r="AP17" s="6"/>
-      <c r="AQ17" s="13"/>
-    </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ17" s="6"/>
+      <c r="AR17" s="13"/>
+    </row>
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="16"/>
@@ -1655,9 +1681,10 @@
       <c r="AN18" s="6"/>
       <c r="AO18" s="6"/>
       <c r="AP18" s="6"/>
-      <c r="AQ18" s="13"/>
-    </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ18" s="6"/>
+      <c r="AR18" s="13"/>
+    </row>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="16"/>
@@ -1700,9 +1727,10 @@
       <c r="AN19" s="6"/>
       <c r="AO19" s="6"/>
       <c r="AP19" s="6"/>
-      <c r="AQ19" s="13"/>
-    </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ19" s="6"/>
+      <c r="AR19" s="13"/>
+    </row>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="16"/>
@@ -1745,9 +1773,10 @@
       <c r="AN20" s="6"/>
       <c r="AO20" s="6"/>
       <c r="AP20" s="6"/>
-      <c r="AQ20" s="13"/>
-    </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ20" s="6"/>
+      <c r="AR20" s="13"/>
+    </row>
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="16"/>
@@ -1790,9 +1819,10 @@
       <c r="AN21" s="6"/>
       <c r="AO21" s="6"/>
       <c r="AP21" s="6"/>
-      <c r="AQ21" s="13"/>
-    </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ21" s="6"/>
+      <c r="AR21" s="13"/>
+    </row>
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="16"/>
@@ -1835,9 +1865,10 @@
       <c r="AN22" s="6"/>
       <c r="AO22" s="6"/>
       <c r="AP22" s="6"/>
-      <c r="AQ22" s="13"/>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ22" s="6"/>
+      <c r="AR22" s="13"/>
+    </row>
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="16"/>
@@ -1880,9 +1911,10 @@
       <c r="AN23" s="6"/>
       <c r="AO23" s="6"/>
       <c r="AP23" s="6"/>
-      <c r="AQ23" s="13"/>
-    </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ23" s="6"/>
+      <c r="AR23" s="13"/>
+    </row>
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="16"/>
@@ -1925,9 +1957,10 @@
       <c r="AN24" s="6"/>
       <c r="AO24" s="6"/>
       <c r="AP24" s="6"/>
-      <c r="AQ24" s="13"/>
-    </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ24" s="6"/>
+      <c r="AR24" s="13"/>
+    </row>
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="16"/>
@@ -1970,9 +2003,10 @@
       <c r="AN25" s="6"/>
       <c r="AO25" s="6"/>
       <c r="AP25" s="6"/>
-      <c r="AQ25" s="13"/>
-    </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ25" s="6"/>
+      <c r="AR25" s="13"/>
+    </row>
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="16"/>
@@ -2015,9 +2049,10 @@
       <c r="AN26" s="6"/>
       <c r="AO26" s="6"/>
       <c r="AP26" s="6"/>
-      <c r="AQ26" s="13"/>
-    </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ26" s="6"/>
+      <c r="AR26" s="13"/>
+    </row>
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="16"/>
@@ -2060,9 +2095,10 @@
       <c r="AN27" s="6"/>
       <c r="AO27" s="6"/>
       <c r="AP27" s="6"/>
-      <c r="AQ27" s="13"/>
-    </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ27" s="6"/>
+      <c r="AR27" s="13"/>
+    </row>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="16"/>
@@ -2105,9 +2141,10 @@
       <c r="AN28" s="6"/>
       <c r="AO28" s="6"/>
       <c r="AP28" s="6"/>
-      <c r="AQ28" s="13"/>
-    </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ28" s="6"/>
+      <c r="AR28" s="13"/>
+    </row>
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="16"/>
@@ -2150,9 +2187,10 @@
       <c r="AN29" s="6"/>
       <c r="AO29" s="6"/>
       <c r="AP29" s="6"/>
-      <c r="AQ29" s="13"/>
-    </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ29" s="6"/>
+      <c r="AR29" s="13"/>
+    </row>
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="16"/>
@@ -2195,26 +2233,27 @@
       <c r="AN30" s="6"/>
       <c r="AO30" s="6"/>
       <c r="AP30" s="6"/>
-      <c r="AQ30" s="13"/>
-    </row>
-    <row r="31" spans="1:43" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+      <c r="AQ30" s="6"/>
+      <c r="AR30" s="13"/>
+    </row>
+    <row r="31" spans="1:44" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="40"/>
-      <c r="O31" s="40"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
       <c r="P31" s="31">
         <f>SUM(P$7:P30)</f>
         <v>0</v>
@@ -2319,10 +2358,14 @@
         <f xml:space="preserve"> SUM(AO$7:AO30)</f>
         <v>0</v>
       </c>
-      <c r="AP31" s="20"/>
-      <c r="AQ31" s="19"/>
-    </row>
-    <row r="33" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AP31" s="20">
+        <f xml:space="preserve"> SUM(AP$7:AP30)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ31" s="20"/>
+      <c r="AR31" s="19"/>
+    </row>
+    <row r="33" spans="3:44" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -2364,10 +2407,11 @@
       <c r="AO33" s="1"/>
       <c r="AP33" s="1"/>
       <c r="AQ33" s="1"/>
+      <c r="AR33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:AQ1"/>
+    <mergeCell ref="A1:AR1"/>
     <mergeCell ref="A31:O31"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>

</xml_diff>

<commit_message>
ds HDSC: thêm cột {masothue, masothueBH}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon_Gara.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon_Gara.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Tên khách hàng</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Giảm trừ Bảo hiểm</t>
+  </si>
+  <si>
+    <t>Mã số thuế</t>
+  </si>
+  <si>
+    <t>Mã số thuế BH</t>
   </si>
 </sst>
 </file>
@@ -289,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -384,6 +390,9 @@
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -717,12 +726,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS33"/>
+  <dimension ref="A1:AU33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,83 +742,85 @@
     <col min="5" max="5" width="19.7109375" style="14" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" style="14" customWidth="1"/>
     <col min="7" max="7" width="21.140625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" style="9" customWidth="1"/>
-    <col min="13" max="13" width="29" style="9" customWidth="1"/>
-    <col min="14" max="15" width="24.140625" style="9" customWidth="1"/>
-    <col min="16" max="16" width="27.42578125" style="29" customWidth="1"/>
-    <col min="17" max="18" width="24.42578125" style="29" customWidth="1"/>
-    <col min="19" max="20" width="18" style="7" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="7" customWidth="1"/>
-    <col min="22" max="23" width="18.140625" style="7" customWidth="1"/>
-    <col min="24" max="24" width="19.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="19.140625" style="7" customWidth="1"/>
-    <col min="28" max="28" width="31" style="7" customWidth="1"/>
-    <col min="29" max="29" width="29.7109375" style="7" customWidth="1"/>
-    <col min="30" max="30" width="22" style="7" customWidth="1"/>
-    <col min="31" max="31" width="23.42578125" style="7" customWidth="1"/>
-    <col min="32" max="32" width="24.140625" style="7" customWidth="1"/>
-    <col min="33" max="33" width="22.5703125" style="7" customWidth="1"/>
-    <col min="34" max="34" width="25.7109375" style="7" customWidth="1"/>
-    <col min="35" max="41" width="19.140625" style="7" customWidth="1"/>
-    <col min="42" max="43" width="18.140625" style="7" customWidth="1"/>
-    <col min="44" max="44" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="9" width="17.140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="32.140625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" style="9" customWidth="1"/>
+    <col min="13" max="14" width="29.7109375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="29" style="9" customWidth="1"/>
+    <col min="16" max="17" width="24.140625" style="9" customWidth="1"/>
+    <col min="18" max="18" width="27.42578125" style="29" customWidth="1"/>
+    <col min="19" max="20" width="24.42578125" style="29" customWidth="1"/>
+    <col min="21" max="22" width="18" style="7" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" style="7" customWidth="1"/>
+    <col min="24" max="25" width="18.140625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="19.140625" style="7" customWidth="1"/>
+    <col min="30" max="30" width="31" style="7" customWidth="1"/>
+    <col min="31" max="31" width="29.7109375" style="7" customWidth="1"/>
+    <col min="32" max="32" width="22" style="7" customWidth="1"/>
+    <col min="33" max="33" width="23.42578125" style="7" customWidth="1"/>
+    <col min="34" max="34" width="24.140625" style="7" customWidth="1"/>
+    <col min="35" max="35" width="22.5703125" style="7" customWidth="1"/>
+    <col min="36" max="36" width="25.7109375" style="7" customWidth="1"/>
+    <col min="37" max="43" width="19.140625" style="7" customWidth="1"/>
+    <col min="44" max="45" width="18.140625" style="7" customWidth="1"/>
+    <col min="46" max="46" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:47" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="39"/>
-      <c r="AG1" s="39"/>
-      <c r="AH1" s="39"/>
-      <c r="AI1" s="39"/>
-      <c r="AJ1" s="39"/>
-      <c r="AK1" s="39"/>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="39"/>
-      <c r="AN1" s="39"/>
-      <c r="AO1" s="39"/>
-      <c r="AP1" s="39"/>
-      <c r="AQ1" s="39"/>
-      <c r="AR1" s="39"/>
-      <c r="AS1" s="5"/>
-    </row>
-    <row r="2" spans="1:45" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
+      <c r="AK1" s="40"/>
+      <c r="AL1" s="40"/>
+      <c r="AM1" s="40"/>
+      <c r="AN1" s="40"/>
+      <c r="AO1" s="40"/>
+      <c r="AP1" s="40"/>
+      <c r="AQ1" s="40"/>
+      <c r="AR1" s="40"/>
+      <c r="AS1" s="40"/>
+      <c r="AT1" s="40"/>
+      <c r="AU1" s="5"/>
+    </row>
+    <row r="2" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="22"/>
       <c r="C2" s="18"/>
@@ -818,45 +829,47 @@
       <c r="F2" s="26"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="27"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="35"/>
       <c r="L2" s="27"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="23"/>
       <c r="R2" s="28"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="35"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="38"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="33"/>
       <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
+      <c r="AE2" s="38"/>
       <c r="AF2" s="36"/>
       <c r="AG2" s="36"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="35"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="35"/>
       <c r="AM2" s="25"/>
-      <c r="AN2" s="35"/>
+      <c r="AN2" s="25"/>
       <c r="AO2" s="25"/>
-      <c r="AP2" s="23"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="18"/>
-      <c r="AS2" s="5"/>
-    </row>
-    <row r="3" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP2" s="35"/>
+      <c r="AQ2" s="25"/>
+      <c r="AR2" s="23"/>
+      <c r="AS2" s="34"/>
+      <c r="AT2" s="18"/>
+      <c r="AU2" s="5"/>
+    </row>
+    <row r="3" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>13</v>
       </c>
@@ -867,45 +880,47 @@
       <c r="F3" s="21"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="27"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="35"/>
       <c r="L3" s="27"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="23"/>
       <c r="R3" s="28"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="35"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
       <c r="U3" s="18"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="27"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="33"/>
-      <c r="AB3" s="36"/>
-      <c r="AC3" s="38"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="33"/>
       <c r="AD3" s="36"/>
-      <c r="AE3" s="36"/>
+      <c r="AE3" s="38"/>
       <c r="AF3" s="36"/>
       <c r="AG3" s="36"/>
-      <c r="AH3" s="33"/>
-      <c r="AI3" s="33"/>
-      <c r="AJ3" s="35"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
+      <c r="AH3" s="36"/>
+      <c r="AI3" s="36"/>
+      <c r="AJ3" s="33"/>
+      <c r="AK3" s="33"/>
+      <c r="AL3" s="35"/>
       <c r="AM3" s="25"/>
-      <c r="AN3" s="35"/>
+      <c r="AN3" s="25"/>
       <c r="AO3" s="25"/>
-      <c r="AP3" s="23"/>
-      <c r="AQ3" s="34"/>
-      <c r="AR3" s="18"/>
-      <c r="AS3" s="5"/>
-    </row>
-    <row r="4" spans="1:45" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP3" s="35"/>
+      <c r="AQ3" s="25"/>
+      <c r="AR3" s="23"/>
+      <c r="AS3" s="34"/>
+      <c r="AT3" s="18"/>
+      <c r="AU3" s="5"/>
+    </row>
+    <row r="4" spans="1:47" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
@@ -916,45 +931,47 @@
       <c r="F4" s="21"/>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="27"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="35"/>
       <c r="L4" s="27"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="23"/>
       <c r="R4" s="28"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="35"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
       <c r="U4" s="18"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="33"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="38"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="33"/>
       <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
+      <c r="AE4" s="38"/>
       <c r="AF4" s="36"/>
       <c r="AG4" s="36"/>
-      <c r="AH4" s="33"/>
-      <c r="AI4" s="33"/>
-      <c r="AJ4" s="35"/>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="36"/>
+      <c r="AJ4" s="33"/>
+      <c r="AK4" s="33"/>
+      <c r="AL4" s="35"/>
       <c r="AM4" s="25"/>
-      <c r="AN4" s="35"/>
+      <c r="AN4" s="25"/>
       <c r="AO4" s="25"/>
-      <c r="AP4" s="23"/>
-      <c r="AQ4" s="34"/>
-      <c r="AR4" s="18"/>
-      <c r="AS4" s="5"/>
-    </row>
-    <row r="5" spans="1:45" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP4" s="35"/>
+      <c r="AQ4" s="25"/>
+      <c r="AR4" s="23"/>
+      <c r="AS4" s="34"/>
+      <c r="AT4" s="18"/>
+      <c r="AU4" s="5"/>
+    </row>
+    <row r="5" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -997,8 +1014,10 @@
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
-    </row>
-    <row r="6" spans="1:45" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+    </row>
+    <row r="6" spans="1:47" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1024,115 +1043,121 @@
         <v>4</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="N6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="P6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="Q6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="R6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="S6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="T6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="U6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="V6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="U6" s="4" t="s">
+      <c r="W6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="V6" s="4" t="s">
+      <c r="X6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="W6" s="4" t="s">
+      <c r="Y6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="Z6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="AA6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="Z6" s="4" t="s">
+      <c r="AB6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AA6" s="4" t="s">
+      <c r="AC6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AD6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AC6" s="4" t="s">
+      <c r="AE6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AD6" s="4" t="s">
+      <c r="AF6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AE6" s="4" t="s">
+      <c r="AG6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AF6" s="4" t="s">
+      <c r="AH6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AG6" s="4" t="s">
+      <c r="AI6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AH6" s="4" t="s">
+      <c r="AJ6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AI6" s="4" t="s">
+      <c r="AK6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AJ6" s="4" t="s">
+      <c r="AL6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK6" s="4" t="s">
+      <c r="AM6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AL6" s="4" t="s">
+      <c r="AN6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AM6" s="4" t="s">
+      <c r="AO6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AN6" s="4" t="s">
+      <c r="AP6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AO6" s="4" t="s">
+      <c r="AQ6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AP6" s="4" t="s">
+      <c r="AR6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AQ6" s="4" t="s">
+      <c r="AS6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AR6" s="10" t="s">
+      <c r="AT6" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="16"/>
@@ -1141,18 +1166,18 @@
       <c r="F7" s="16"/>
       <c r="G7" s="11"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="11"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
       <c r="R7" s="30"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
@@ -1176,9 +1201,11 @@
       <c r="AO7" s="6"/>
       <c r="AP7" s="6"/>
       <c r="AQ7" s="6"/>
-      <c r="AR7" s="13"/>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AR7" s="6"/>
+      <c r="AS7" s="6"/>
+      <c r="AT7" s="13"/>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="16"/>
@@ -1187,18 +1214,18 @@
       <c r="F8" s="16"/>
       <c r="G8" s="11"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
       <c r="R8" s="30"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
@@ -1222,9 +1249,11 @@
       <c r="AO8" s="6"/>
       <c r="AP8" s="6"/>
       <c r="AQ8" s="6"/>
-      <c r="AR8" s="13"/>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AR8" s="6"/>
+      <c r="AS8" s="6"/>
+      <c r="AT8" s="13"/>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="16"/>
@@ -1233,18 +1262,18 @@
       <c r="F9" s="16"/>
       <c r="G9" s="11"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="11"/>
+      <c r="I9" s="13"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
       <c r="R9" s="30"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -1268,9 +1297,11 @@
       <c r="AO9" s="6"/>
       <c r="AP9" s="6"/>
       <c r="AQ9" s="6"/>
-      <c r="AR9" s="13"/>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AR9" s="6"/>
+      <c r="AS9" s="6"/>
+      <c r="AT9" s="13"/>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="16"/>
@@ -1279,18 +1310,18 @@
       <c r="F10" s="16"/>
       <c r="G10" s="11"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="13"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
       <c r="R10" s="30"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
@@ -1314,9 +1345,11 @@
       <c r="AO10" s="6"/>
       <c r="AP10" s="6"/>
       <c r="AQ10" s="6"/>
-      <c r="AR10" s="13"/>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="6"/>
+      <c r="AT10" s="13"/>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="16"/>
@@ -1325,18 +1358,18 @@
       <c r="F11" s="16"/>
       <c r="G11" s="11"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
       <c r="R11" s="30"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
@@ -1360,9 +1393,11 @@
       <c r="AO11" s="6"/>
       <c r="AP11" s="6"/>
       <c r="AQ11" s="6"/>
-      <c r="AR11" s="13"/>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AR11" s="6"/>
+      <c r="AS11" s="6"/>
+      <c r="AT11" s="13"/>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="16"/>
@@ -1371,18 +1406,18 @@
       <c r="F12" s="16"/>
       <c r="G12" s="11"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="11"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
       <c r="R12" s="30"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
@@ -1406,9 +1441,11 @@
       <c r="AO12" s="6"/>
       <c r="AP12" s="6"/>
       <c r="AQ12" s="6"/>
-      <c r="AR12" s="13"/>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AR12" s="6"/>
+      <c r="AS12" s="6"/>
+      <c r="AT12" s="13"/>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="16"/>
@@ -1417,18 +1454,18 @@
       <c r="F13" s="16"/>
       <c r="G13" s="11"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="11"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
       <c r="R13" s="30"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
@@ -1452,9 +1489,11 @@
       <c r="AO13" s="6"/>
       <c r="AP13" s="6"/>
       <c r="AQ13" s="6"/>
-      <c r="AR13" s="13"/>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AR13" s="6"/>
+      <c r="AS13" s="6"/>
+      <c r="AT13" s="13"/>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="16"/>
@@ -1463,18 +1502,18 @@
       <c r="F14" s="16"/>
       <c r="G14" s="11"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="11"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
       <c r="R14" s="30"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
@@ -1498,9 +1537,11 @@
       <c r="AO14" s="6"/>
       <c r="AP14" s="6"/>
       <c r="AQ14" s="6"/>
-      <c r="AR14" s="13"/>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AR14" s="6"/>
+      <c r="AS14" s="6"/>
+      <c r="AT14" s="13"/>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="16"/>
@@ -1509,18 +1550,18 @@
       <c r="F15" s="16"/>
       <c r="G15" s="11"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="11"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
       <c r="R15" s="30"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
@@ -1544,9 +1585,11 @@
       <c r="AO15" s="6"/>
       <c r="AP15" s="6"/>
       <c r="AQ15" s="6"/>
-      <c r="AR15" s="13"/>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AR15" s="6"/>
+      <c r="AS15" s="6"/>
+      <c r="AT15" s="13"/>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="16"/>
@@ -1555,18 +1598,18 @@
       <c r="F16" s="16"/>
       <c r="G16" s="11"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="11"/>
+      <c r="I16" s="13"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
       <c r="R16" s="30"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
@@ -1590,9 +1633,11 @@
       <c r="AO16" s="6"/>
       <c r="AP16" s="6"/>
       <c r="AQ16" s="6"/>
-      <c r="AR16" s="13"/>
-    </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR16" s="6"/>
+      <c r="AS16" s="6"/>
+      <c r="AT16" s="13"/>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="16"/>
@@ -1601,18 +1646,18 @@
       <c r="F17" s="16"/>
       <c r="G17" s="11"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="11"/>
+      <c r="I17" s="13"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
       <c r="R17" s="30"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
@@ -1636,9 +1681,11 @@
       <c r="AO17" s="6"/>
       <c r="AP17" s="6"/>
       <c r="AQ17" s="6"/>
-      <c r="AR17" s="13"/>
-    </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR17" s="6"/>
+      <c r="AS17" s="6"/>
+      <c r="AT17" s="13"/>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="16"/>
@@ -1647,18 +1694,18 @@
       <c r="F18" s="16"/>
       <c r="G18" s="11"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="11"/>
+      <c r="I18" s="13"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
       <c r="R18" s="30"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
@@ -1682,9 +1729,11 @@
       <c r="AO18" s="6"/>
       <c r="AP18" s="6"/>
       <c r="AQ18" s="6"/>
-      <c r="AR18" s="13"/>
-    </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR18" s="6"/>
+      <c r="AS18" s="6"/>
+      <c r="AT18" s="13"/>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="16"/>
@@ -1693,18 +1742,18 @@
       <c r="F19" s="16"/>
       <c r="G19" s="11"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="11"/>
+      <c r="I19" s="13"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
       <c r="R19" s="30"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
@@ -1728,9 +1777,11 @@
       <c r="AO19" s="6"/>
       <c r="AP19" s="6"/>
       <c r="AQ19" s="6"/>
-      <c r="AR19" s="13"/>
-    </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR19" s="6"/>
+      <c r="AS19" s="6"/>
+      <c r="AT19" s="13"/>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="16"/>
@@ -1739,18 +1790,18 @@
       <c r="F20" s="16"/>
       <c r="G20" s="11"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="11"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
       <c r="R20" s="30"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
@@ -1774,9 +1825,11 @@
       <c r="AO20" s="6"/>
       <c r="AP20" s="6"/>
       <c r="AQ20" s="6"/>
-      <c r="AR20" s="13"/>
-    </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR20" s="6"/>
+      <c r="AS20" s="6"/>
+      <c r="AT20" s="13"/>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="16"/>
@@ -1785,18 +1838,18 @@
       <c r="F21" s="16"/>
       <c r="G21" s="11"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="11"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
       <c r="R21" s="30"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
@@ -1820,9 +1873,11 @@
       <c r="AO21" s="6"/>
       <c r="AP21" s="6"/>
       <c r="AQ21" s="6"/>
-      <c r="AR21" s="13"/>
-    </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR21" s="6"/>
+      <c r="AS21" s="6"/>
+      <c r="AT21" s="13"/>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="16"/>
@@ -1831,18 +1886,18 @@
       <c r="F22" s="16"/>
       <c r="G22" s="11"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="11"/>
+      <c r="I22" s="13"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
       <c r="R22" s="30"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
@@ -1866,9 +1921,11 @@
       <c r="AO22" s="6"/>
       <c r="AP22" s="6"/>
       <c r="AQ22" s="6"/>
-      <c r="AR22" s="13"/>
-    </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR22" s="6"/>
+      <c r="AS22" s="6"/>
+      <c r="AT22" s="13"/>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="16"/>
@@ -1877,18 +1934,18 @@
       <c r="F23" s="16"/>
       <c r="G23" s="11"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="11"/>
+      <c r="I23" s="13"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
       <c r="R23" s="30"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
@@ -1912,9 +1969,11 @@
       <c r="AO23" s="6"/>
       <c r="AP23" s="6"/>
       <c r="AQ23" s="6"/>
-      <c r="AR23" s="13"/>
-    </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR23" s="6"/>
+      <c r="AS23" s="6"/>
+      <c r="AT23" s="13"/>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="16"/>
@@ -1923,18 +1982,18 @@
       <c r="F24" s="16"/>
       <c r="G24" s="11"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="11"/>
+      <c r="I24" s="13"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
       <c r="R24" s="30"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
@@ -1958,9 +2017,11 @@
       <c r="AO24" s="6"/>
       <c r="AP24" s="6"/>
       <c r="AQ24" s="6"/>
-      <c r="AR24" s="13"/>
-    </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR24" s="6"/>
+      <c r="AS24" s="6"/>
+      <c r="AT24" s="13"/>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="16"/>
@@ -1969,18 +2030,18 @@
       <c r="F25" s="16"/>
       <c r="G25" s="11"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="11"/>
+      <c r="I25" s="13"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
       <c r="O25" s="11"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
       <c r="R25" s="30"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
@@ -2004,9 +2065,11 @@
       <c r="AO25" s="6"/>
       <c r="AP25" s="6"/>
       <c r="AQ25" s="6"/>
-      <c r="AR25" s="13"/>
-    </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR25" s="6"/>
+      <c r="AS25" s="6"/>
+      <c r="AT25" s="13"/>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="16"/>
@@ -2015,18 +2078,18 @@
       <c r="F26" s="16"/>
       <c r="G26" s="11"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="11"/>
+      <c r="I26" s="13"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
       <c r="O26" s="11"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
       <c r="R26" s="30"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
@@ -2050,9 +2113,11 @@
       <c r="AO26" s="6"/>
       <c r="AP26" s="6"/>
       <c r="AQ26" s="6"/>
-      <c r="AR26" s="13"/>
-    </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR26" s="6"/>
+      <c r="AS26" s="6"/>
+      <c r="AT26" s="13"/>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="16"/>
@@ -2061,18 +2126,18 @@
       <c r="F27" s="16"/>
       <c r="G27" s="11"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="11"/>
+      <c r="I27" s="13"/>
       <c r="J27" s="11"/>
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
       <c r="R27" s="30"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
@@ -2096,9 +2161,11 @@
       <c r="AO27" s="6"/>
       <c r="AP27" s="6"/>
       <c r="AQ27" s="6"/>
-      <c r="AR27" s="13"/>
-    </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR27" s="6"/>
+      <c r="AS27" s="6"/>
+      <c r="AT27" s="13"/>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="16"/>
@@ -2107,18 +2174,18 @@
       <c r="F28" s="16"/>
       <c r="G28" s="11"/>
       <c r="H28" s="13"/>
-      <c r="I28" s="11"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
       <c r="N28" s="11"/>
       <c r="O28" s="11"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
       <c r="R28" s="30"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
@@ -2142,9 +2209,11 @@
       <c r="AO28" s="6"/>
       <c r="AP28" s="6"/>
       <c r="AQ28" s="6"/>
-      <c r="AR28" s="13"/>
-    </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR28" s="6"/>
+      <c r="AS28" s="6"/>
+      <c r="AT28" s="13"/>
+    </row>
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="16"/>
@@ -2153,18 +2222,18 @@
       <c r="F29" s="16"/>
       <c r="G29" s="11"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="11"/>
+      <c r="I29" s="13"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
       <c r="R29" s="30"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
       <c r="W29" s="6"/>
@@ -2188,9 +2257,11 @@
       <c r="AO29" s="6"/>
       <c r="AP29" s="6"/>
       <c r="AQ29" s="6"/>
-      <c r="AR29" s="13"/>
-    </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR29" s="6"/>
+      <c r="AS29" s="6"/>
+      <c r="AT29" s="13"/>
+    </row>
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="16"/>
@@ -2199,18 +2270,18 @@
       <c r="F30" s="16"/>
       <c r="G30" s="11"/>
       <c r="H30" s="13"/>
-      <c r="I30" s="11"/>
+      <c r="I30" s="13"/>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
       <c r="N30" s="11"/>
       <c r="O30" s="11"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
       <c r="R30" s="30"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
@@ -2234,43 +2305,39 @@
       <c r="AO30" s="6"/>
       <c r="AP30" s="6"/>
       <c r="AQ30" s="6"/>
-      <c r="AR30" s="13"/>
-    </row>
-    <row r="31" spans="1:44" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="40" t="s">
+      <c r="AR30" s="6"/>
+      <c r="AS30" s="6"/>
+      <c r="AT30" s="13"/>
+    </row>
+    <row r="31" spans="1:46" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="41"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="31">
-        <f>SUM(P$7:P30)</f>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="31">
-        <f>SUM(Q$7:Q30)</f>
-        <v>0</v>
-      </c>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="42"/>
+      <c r="Q31" s="42"/>
       <c r="R31" s="31">
         <f>SUM(R$7:R30)</f>
         <v>0</v>
       </c>
-      <c r="S31" s="20">
+      <c r="S31" s="31">
         <f>SUM(S$7:S30)</f>
         <v>0</v>
       </c>
-      <c r="T31" s="20">
+      <c r="T31" s="31">
         <f>SUM(T$7:T30)</f>
         <v>0</v>
       </c>
@@ -2279,11 +2346,11 @@
         <v>0</v>
       </c>
       <c r="V31" s="20">
-        <f xml:space="preserve"> SUM(V$7:V30)</f>
+        <f>SUM(V$7:V30)</f>
         <v>0</v>
       </c>
       <c r="W31" s="20">
-        <f xml:space="preserve"> SUM(W$7:W30)</f>
+        <f>SUM(W$7:W30)</f>
         <v>0</v>
       </c>
       <c r="X31" s="20">
@@ -2362,10 +2429,18 @@
         <f xml:space="preserve"> SUM(AP$7:AP30)</f>
         <v>0</v>
       </c>
-      <c r="AQ31" s="20"/>
-      <c r="AR31" s="19"/>
-    </row>
-    <row r="33" spans="3:44" x14ac:dyDescent="0.25">
+      <c r="AQ31" s="20">
+        <f xml:space="preserve"> SUM(AQ$7:AQ30)</f>
+        <v>0</v>
+      </c>
+      <c r="AR31" s="20">
+        <f xml:space="preserve"> SUM(AR$7:AR30)</f>
+        <v>0</v>
+      </c>
+      <c r="AS31" s="20"/>
+      <c r="AT31" s="19"/>
+    </row>
+    <row r="33" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -2379,11 +2454,11 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="32"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
       <c r="R33" s="32"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
@@ -2408,11 +2483,13 @@
       <c r="AP33" s="1"/>
       <c r="AQ33" s="1"/>
       <c r="AR33" s="1"/>
+      <c r="AS33" s="1"/>
+      <c r="AT33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:AR1"/>
-    <mergeCell ref="A31:O31"/>
+    <mergeCell ref="A1:AT1"/>
+    <mergeCell ref="A31:Q31"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>